<commit_message>
extend warehouse new module
</commit_message>
<xml_diff>
--- a/td_template_import/other_warehouses/59.xlsx
+++ b/td_template_import/other_warehouses/59.xlsx
@@ -19,55 +19,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
-  <si>
-    <t>Mã hàng</t>
-  </si>
-  <si>
-    <t>Tên hàng</t>
-  </si>
-  <si>
-    <t>ĐVT</t>
-  </si>
-  <si>
-    <t>Số lượng 
-kiểm thực</t>
-  </si>
-  <si>
-    <t>BANGDINH1F</t>
-  </si>
-  <si>
-    <t>Băng dính trắng 1cm</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="52">
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Bản</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Băng dính trắng</t>
+  </si>
+  <si>
+    <t>1cm</t>
   </si>
   <si>
     <t>Cuộn</t>
   </si>
   <si>
-    <t>BANGDINH2M0.5F</t>
-  </si>
-  <si>
-    <t>Băng dính 2 mặt 0.5 phân</t>
-  </si>
-  <si>
-    <t>BANGDINH2M1F</t>
-  </si>
-  <si>
-    <t>Băng dính 2 mặt 1 phân ( 1 cây/30 cuộn)</t>
-  </si>
-  <si>
-    <t>BANGDINH5F</t>
-  </si>
-  <si>
-    <t>Băng dính 5 cm</t>
-  </si>
-  <si>
-    <t>Cây</t>
-  </si>
-  <si>
-    <t>BANGDINHDANTHUNG</t>
-  </si>
-  <si>
-    <t>Băng dính dán thùng ( 1 cây / 6 cuộn)</t>
+    <t>Băng dính 2 mặt</t>
+  </si>
+  <si>
+    <t>0.5cm</t>
+  </si>
+  <si>
+    <t>5cm</t>
+  </si>
+  <si>
+    <t>4.8cm</t>
+  </si>
+  <si>
+    <t>Băng dính góc</t>
+  </si>
+  <si>
+    <t>1.9cm</t>
+  </si>
+  <si>
+    <t>Bóng kính</t>
+  </si>
+  <si>
+    <t>50x70</t>
+  </si>
+  <si>
+    <t>Tờ</t>
+  </si>
+  <si>
+    <t>DVT</t>
+  </si>
+  <si>
+    <t>Loại</t>
+  </si>
+  <si>
+    <t>Hoàn thiện</t>
+  </si>
+  <si>
+    <t>Bán tự động</t>
+  </si>
+  <si>
+    <t>Tự động</t>
+  </si>
+  <si>
+    <t>Chun</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Gân</t>
+  </si>
+  <si>
+    <t>Hộp</t>
+  </si>
+  <si>
+    <t>Cái</t>
+  </si>
+  <si>
+    <t>Lọ nhỏ keo</t>
+  </si>
+  <si>
+    <t>Lọ</t>
+  </si>
+  <si>
+    <t>DÂY TẾT NHÊ 4</t>
+  </si>
+  <si>
+    <t>Dây tết vàng nhỏ</t>
+  </si>
+  <si>
+    <t>35cm</t>
+  </si>
+  <si>
+    <t>Đôi</t>
+  </si>
+  <si>
+    <t>DÂY DÙ NHÊ 4</t>
+  </si>
+  <si>
+    <t>Dây đen nhỏ</t>
+  </si>
+  <si>
+    <t>Dây đỏ nhỏ</t>
+  </si>
+  <si>
+    <t>DÂY DÙ NHÊ 5</t>
+  </si>
+  <si>
+    <t>Dây nâu to</t>
+  </si>
+  <si>
+    <t>DÂY RUY BĂNG VẢI</t>
+  </si>
+  <si>
+    <t>Dây Ruy băng 048</t>
+  </si>
+  <si>
+    <t>Dây Ruy băng  049</t>
+  </si>
+  <si>
+    <t>Dây Ruy băng  051</t>
+  </si>
+  <si>
+    <t>Dây Ruy băng  052</t>
+  </si>
+  <si>
+    <t>Dây Ruy băng  053</t>
+  </si>
+  <si>
+    <t>DâyRuy băng 054</t>
+  </si>
+  <si>
+    <t>Dây Ruy băng 055</t>
+  </si>
+  <si>
+    <t>Dây  Ruy băng  056</t>
+  </si>
+  <si>
+    <t>Dây  Ruy băng 057</t>
+  </si>
+  <si>
+    <t>Dây  Ruy băng  060</t>
+  </si>
+  <si>
+    <t>DÂY XOẮN NHÊ 5</t>
+  </si>
+  <si>
+    <t>Dây xoắn đỏ to</t>
+  </si>
+  <si>
+    <t>Dây xoắn trắng to</t>
+  </si>
+  <si>
+    <t>Dây dù xanh nhỏ</t>
+  </si>
+  <si>
+    <t>Dây xoắn xanh to</t>
   </si>
 </sst>
 </file>
@@ -75,8 +182,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -95,14 +202,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Microsoft Sans Serif"/>
@@ -112,6 +211,13 @@
       <sz val="8"/>
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -146,21 +252,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -177,26 +268,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -478,110 +591,569 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="6">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="8">
+        <v>18700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="8">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="8">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="8">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="8">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="8">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="8">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4">
-        <v>121</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>